<commit_message>
- GBIF R script - visitor log update
</commit_message>
<xml_diff>
--- a/visitors/Ornithology visitor log.xlsx
+++ b/visitors/Ornithology visitor log.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Desktop\nhm_ornithology\visitors\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Documents\nhm_ornithology\visitors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E58303-3995-46D7-BBD6-17086A6A8103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB1B492A-9123-4614-AACE-97FA3CE58FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19470" yWindow="495" windowWidth="16845" windowHeight="14985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ongoing" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ongoing!$F$1:$F$1011</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ongoing!$F$1:$F$1018</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1982" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2184" uniqueCount="617">
   <si>
     <t>VISITOR</t>
   </si>
@@ -1697,6 +1697,201 @@
   </si>
   <si>
     <t>Collection tour (12 students)</t>
+  </si>
+  <si>
+    <t>Sam Tayag</t>
+  </si>
+  <si>
+    <t>SAMO Youth Tour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMO </t>
+  </si>
+  <si>
+    <t>Whitney + Russell tour</t>
+  </si>
+  <si>
+    <t>Leslie's guests</t>
+  </si>
+  <si>
+    <t>Vera Ting</t>
+  </si>
+  <si>
+    <t>CLO</t>
+  </si>
+  <si>
+    <t>Artist working on birds</t>
+  </si>
+  <si>
+    <t>Samantha Rutledge</t>
+  </si>
+  <si>
+    <t>Measuring starlings</t>
+  </si>
+  <si>
+    <t>Phil Koken</t>
+  </si>
+  <si>
+    <t>Imaging extinct birds (Auk)</t>
+  </si>
+  <si>
+    <t>Madeline Cass</t>
+  </si>
+  <si>
+    <t>Imaging extinct birds + skeletons</t>
+  </si>
+  <si>
+    <t>BTS Tour</t>
+  </si>
+  <si>
+    <t>Collections tour</t>
+  </si>
+  <si>
+    <t>Chapman University tour</t>
+  </si>
+  <si>
+    <t>Pierce College tour</t>
+  </si>
+  <si>
+    <t>Pierce College</t>
+  </si>
+  <si>
+    <t>Ian McAllan</t>
+  </si>
+  <si>
+    <t>Macquarie University</t>
+  </si>
+  <si>
+    <t>Measuring Frigatebirds</t>
+  </si>
+  <si>
+    <t>Philip Lavretsky</t>
+  </si>
+  <si>
+    <t>UT El Paso</t>
+  </si>
+  <si>
+    <t>Measuring and imaging ducks</t>
+  </si>
+  <si>
+    <t>Clinton Francis</t>
+  </si>
+  <si>
+    <t>California Polytechnic State University SLO</t>
+  </si>
+  <si>
+    <t>measure eye geometries from skeletons</t>
+  </si>
+  <si>
+    <t>LMU Class tour</t>
+  </si>
+  <si>
+    <t>LMU</t>
+  </si>
+  <si>
+    <t>Andy Birch</t>
+  </si>
+  <si>
+    <t>Katie Hendeson</t>
+  </si>
+  <si>
+    <t>El Camino College Field Zoology</t>
+  </si>
+  <si>
+    <t>Observing pipits</t>
+  </si>
+  <si>
+    <t>LA Birders</t>
+  </si>
+  <si>
+    <t>Observing swifts</t>
+  </si>
+  <si>
+    <t>U North Carolina</t>
+  </si>
+  <si>
+    <t>Observing bird skeletons</t>
+  </si>
+  <si>
+    <t>Matthew Mitchell</t>
+  </si>
+  <si>
+    <t>Kaiya Provost</t>
+  </si>
+  <si>
+    <t>Institute of Zoology, London Zoo</t>
+  </si>
+  <si>
+    <t>Measuring extinct in wild, captive birds</t>
+  </si>
+  <si>
+    <t>Project Phoenix tours</t>
+  </si>
+  <si>
+    <t>NHM/UCLA</t>
+  </si>
+  <si>
+    <t>Stacia Novy</t>
+  </si>
+  <si>
+    <t>Southern Illinois University Edwardsville</t>
+  </si>
+  <si>
+    <t>Measuring Buteogallus specimens</t>
+  </si>
+  <si>
+    <t>Nancy Chiu</t>
+  </si>
+  <si>
+    <t>Observing gray partridge</t>
+  </si>
+  <si>
+    <t>Michael Bailey</t>
+  </si>
+  <si>
+    <t>Observing green pheasant, western tanager, etc.</t>
+  </si>
+  <si>
+    <t>Measuring least terns</t>
+  </si>
+  <si>
+    <t>AFBER class tour</t>
+  </si>
+  <si>
+    <t>Cal Poly Pomona tour</t>
+  </si>
+  <si>
+    <t>USC Visit</t>
+  </si>
+  <si>
+    <t>Ad agency bird tour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Collections  </t>
+  </si>
+  <si>
+    <t>Visit</t>
+  </si>
+  <si>
+    <t>Artist</t>
+  </si>
+  <si>
+    <t>PNC Bank</t>
+  </si>
+  <si>
+    <t>REA</t>
+  </si>
+  <si>
+    <t>Photographer</t>
+  </si>
+  <si>
+    <t>Researcher</t>
+  </si>
+  <si>
+    <t>AFBER</t>
+  </si>
+  <si>
+    <t>Ad agency</t>
   </si>
 </sst>
 </file>
@@ -1706,11 +1901,25 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1758,6 +1967,12 @@
       <color rgb="FF222222"/>
       <name val="&quot;Google Sans&quot;"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1791,27 +2006,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="15" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="15" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2027,18 +2245,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1011"/>
+  <dimension ref="A1:H1018"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <pane ySplit="1" topLeftCell="A338" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C413" sqref="C413"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="21.8984375" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="42.3984375" customWidth="1"/>
-    <col min="4" max="4" width="25.3984375" customWidth="1"/>
+    <col min="2" max="2" width="10.8984375" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="10.59765625" customWidth="1"/>
     <col min="5" max="5" width="47" customWidth="1"/>
     <col min="6" max="6" width="10.69921875" customWidth="1"/>
     <col min="7" max="28" width="7.59765625" customWidth="1"/>
@@ -9322,6 +9541,9 @@
       <c r="B304" s="5">
         <v>44635</v>
       </c>
+      <c r="C304" t="s">
+        <v>609</v>
+      </c>
       <c r="D304" s="4" t="s">
         <v>547</v>
       </c>
@@ -9343,6 +9565,9 @@
       <c r="B305" s="5">
         <v>44635</v>
       </c>
+      <c r="C305" t="s">
+        <v>609</v>
+      </c>
       <c r="D305" s="4" t="s">
         <v>547</v>
       </c>
@@ -9364,6 +9589,9 @@
       <c r="B306" s="5">
         <v>44635</v>
       </c>
+      <c r="C306" t="s">
+        <v>609</v>
+      </c>
       <c r="D306" s="4" t="s">
         <v>547</v>
       </c>
@@ -10366,6 +10594,9 @@
       <c r="B345" s="5">
         <v>45006</v>
       </c>
+      <c r="C345" s="9" t="s">
+        <v>610</v>
+      </c>
       <c r="D345" s="4" t="s">
         <v>546</v>
       </c>
@@ -10470,7 +10701,9 @@
       <c r="B349" s="11">
         <v>45013</v>
       </c>
-      <c r="C349" s="9"/>
+      <c r="C349" s="9" t="s">
+        <v>610</v>
+      </c>
       <c r="D349" s="4" t="s">
         <v>546</v>
       </c>
@@ -10495,7 +10728,9 @@
       <c r="B350" s="11">
         <v>45014</v>
       </c>
-      <c r="C350" s="9"/>
+      <c r="C350" s="9" t="s">
+        <v>611</v>
+      </c>
       <c r="D350" s="4" t="s">
         <v>547</v>
       </c>
@@ -10520,7 +10755,9 @@
       <c r="B351" s="11">
         <v>45019</v>
       </c>
-      <c r="C351" s="9"/>
+      <c r="C351" s="9" t="s">
+        <v>533</v>
+      </c>
       <c r="D351" s="4" t="s">
         <v>547</v>
       </c>
@@ -10621,6 +10858,9 @@
       <c r="B355" s="5">
         <v>45084</v>
       </c>
+      <c r="C355" s="9" t="s">
+        <v>610</v>
+      </c>
       <c r="D355" s="4" t="s">
         <v>546</v>
       </c>
@@ -10670,6 +10910,9 @@
       <c r="B357" s="5">
         <v>45093</v>
       </c>
+      <c r="C357" t="s">
+        <v>612</v>
+      </c>
       <c r="D357" s="4" t="s">
         <v>545</v>
       </c>
@@ -10828,162 +11071,1133 @@
       </c>
     </row>
     <row r="364" spans="1:8" ht="15.75" customHeight="1">
-      <c r="B364" s="5"/>
+      <c r="A364" t="s">
+        <v>552</v>
+      </c>
+      <c r="B364" s="5">
+        <v>45128</v>
+      </c>
+      <c r="C364" t="s">
+        <v>533</v>
+      </c>
+      <c r="D364" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="E364" t="s">
+        <v>454</v>
+      </c>
+      <c r="F364">
+        <v>2</v>
+      </c>
+      <c r="G364" s="6">
+        <v>2023</v>
+      </c>
     </row>
     <row r="365" spans="1:8" ht="15.75" customHeight="1">
-      <c r="B365" s="5"/>
+      <c r="A365" t="s">
+        <v>553</v>
+      </c>
+      <c r="B365" s="5">
+        <v>45128</v>
+      </c>
+      <c r="C365" t="s">
+        <v>554</v>
+      </c>
+      <c r="D365" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="E365" t="s">
+        <v>454</v>
+      </c>
+      <c r="F365">
+        <v>25</v>
+      </c>
+      <c r="G365" s="6">
+        <v>2023</v>
+      </c>
     </row>
     <row r="366" spans="1:8" ht="15.75" customHeight="1">
-      <c r="B366" s="5"/>
+      <c r="A366" t="s">
+        <v>524</v>
+      </c>
+      <c r="B366" s="5">
+        <v>45135</v>
+      </c>
+      <c r="C366" t="s">
+        <v>525</v>
+      </c>
+      <c r="D366" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="E366" s="6" t="s">
+        <v>526</v>
+      </c>
+      <c r="F366">
+        <v>1</v>
+      </c>
+      <c r="G366">
+        <v>2023</v>
+      </c>
     </row>
     <row r="367" spans="1:8" ht="15.75" customHeight="1">
-      <c r="B367" s="5"/>
+      <c r="A367" t="s">
+        <v>555</v>
+      </c>
+      <c r="B367" s="5">
+        <v>45161</v>
+      </c>
+      <c r="C367" t="s">
+        <v>8</v>
+      </c>
+      <c r="D367" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="E367" t="s">
+        <v>454</v>
+      </c>
+      <c r="F367">
+        <v>5</v>
+      </c>
+      <c r="G367">
+        <v>2023</v>
+      </c>
     </row>
     <row r="368" spans="1:8" ht="15.75" customHeight="1">
-      <c r="B368" s="5"/>
-    </row>
-    <row r="369" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B369" s="5"/>
-    </row>
-    <row r="370" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B370" s="5"/>
-    </row>
-    <row r="371" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B371" s="5"/>
-    </row>
-    <row r="372" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B372" s="5"/>
-    </row>
-    <row r="373" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B373" s="5"/>
-    </row>
-    <row r="374" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B374" s="5"/>
-    </row>
-    <row r="375" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B375" s="5"/>
-    </row>
-    <row r="376" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B376" s="5"/>
-    </row>
-    <row r="377" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B377" s="5"/>
-    </row>
-    <row r="378" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B378" s="5"/>
-    </row>
-    <row r="379" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B379" s="5"/>
-    </row>
-    <row r="380" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B380" s="5"/>
-    </row>
-    <row r="381" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B381" s="5"/>
-    </row>
-    <row r="382" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B382" s="5"/>
-    </row>
-    <row r="383" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B383" s="5"/>
-    </row>
-    <row r="384" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B384" s="5"/>
-    </row>
-    <row r="385" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B385" s="5"/>
-    </row>
-    <row r="386" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B386" s="5"/>
-    </row>
-    <row r="387" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B387" s="5"/>
-    </row>
-    <row r="388" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B388" s="5"/>
-    </row>
-    <row r="389" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B389" s="5"/>
-    </row>
-    <row r="390" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B390" s="5"/>
-    </row>
-    <row r="391" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B391" s="5"/>
-    </row>
-    <row r="392" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B392" s="5"/>
-    </row>
-    <row r="393" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B393" s="5"/>
-    </row>
-    <row r="394" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B394" s="5"/>
-    </row>
-    <row r="395" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B395" s="5"/>
-    </row>
-    <row r="396" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B396" s="5"/>
-    </row>
-    <row r="397" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B397" s="5"/>
-    </row>
-    <row r="398" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B398" s="5"/>
-    </row>
-    <row r="399" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B399" s="5"/>
-    </row>
-    <row r="400" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B400" s="5"/>
-    </row>
-    <row r="401" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B401" s="5"/>
-    </row>
-    <row r="402" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B402" s="5"/>
-    </row>
-    <row r="403" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B403" s="5"/>
-    </row>
-    <row r="404" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B404" s="5"/>
-    </row>
-    <row r="405" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B405" s="5"/>
-    </row>
-    <row r="406" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B406" s="5"/>
-    </row>
-    <row r="407" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B407" s="5"/>
-    </row>
-    <row r="408" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B408" s="5"/>
-    </row>
-    <row r="409" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B409" s="5"/>
-    </row>
-    <row r="410" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B410" s="5"/>
-    </row>
-    <row r="411" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B411" s="5"/>
-    </row>
-    <row r="412" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B412" s="5"/>
-    </row>
-    <row r="413" spans="2:2" ht="15.75" customHeight="1">
+      <c r="A368" t="s">
+        <v>524</v>
+      </c>
+      <c r="B368" s="5">
+        <v>45163</v>
+      </c>
+      <c r="C368" t="s">
+        <v>525</v>
+      </c>
+      <c r="D368" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="E368" s="6" t="s">
+        <v>526</v>
+      </c>
+      <c r="F368">
+        <v>1</v>
+      </c>
+      <c r="G368">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="369" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A369" t="s">
+        <v>571</v>
+      </c>
+      <c r="B369" s="5">
+        <v>45174</v>
+      </c>
+      <c r="C369" t="s">
+        <v>572</v>
+      </c>
+      <c r="D369" s="16" t="s">
+        <v>545</v>
+      </c>
+      <c r="E369" s="17" t="s">
+        <v>573</v>
+      </c>
+      <c r="F369">
+        <v>1</v>
+      </c>
+      <c r="G369">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="370" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A370" t="s">
+        <v>556</v>
+      </c>
+      <c r="B370" s="5">
+        <v>45174</v>
+      </c>
+      <c r="C370" t="s">
+        <v>533</v>
+      </c>
+      <c r="D370" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="E370" t="s">
+        <v>454</v>
+      </c>
+      <c r="F370">
+        <v>4</v>
+      </c>
+      <c r="G370">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="371" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A371" t="s">
+        <v>574</v>
+      </c>
+      <c r="B371" s="5">
+        <v>45181</v>
+      </c>
+      <c r="C371" s="17" t="s">
+        <v>575</v>
+      </c>
+      <c r="D371" s="16" t="s">
+        <v>545</v>
+      </c>
+      <c r="E371" t="s">
+        <v>576</v>
+      </c>
+      <c r="F371">
+        <v>2</v>
+      </c>
+      <c r="G371">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="372" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A372" t="s">
+        <v>577</v>
+      </c>
+      <c r="B372" s="5">
+        <v>45187</v>
+      </c>
+      <c r="C372" s="17" t="s">
+        <v>578</v>
+      </c>
+      <c r="D372" s="16" t="s">
+        <v>545</v>
+      </c>
+      <c r="E372" t="s">
+        <v>579</v>
+      </c>
+      <c r="F372">
+        <v>3</v>
+      </c>
+      <c r="G372">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="373" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A373" t="s">
+        <v>577</v>
+      </c>
+      <c r="B373" s="5">
+        <v>45188</v>
+      </c>
+      <c r="C373" s="17" t="s">
+        <v>578</v>
+      </c>
+      <c r="D373" s="16" t="s">
+        <v>545</v>
+      </c>
+      <c r="E373" t="s">
+        <v>579</v>
+      </c>
+      <c r="F373">
+        <v>3</v>
+      </c>
+      <c r="G373">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="374" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A374" t="s">
+        <v>577</v>
+      </c>
+      <c r="B374" s="5">
+        <v>45189</v>
+      </c>
+      <c r="C374" s="17" t="s">
+        <v>578</v>
+      </c>
+      <c r="D374" s="16" t="s">
+        <v>545</v>
+      </c>
+      <c r="E374" t="s">
+        <v>579</v>
+      </c>
+      <c r="F374">
+        <v>3</v>
+      </c>
+      <c r="G374">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="375" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A375" t="s">
+        <v>557</v>
+      </c>
+      <c r="B375" s="5">
+        <v>45188</v>
+      </c>
+      <c r="C375" t="s">
+        <v>558</v>
+      </c>
+      <c r="D375" s="4" t="s">
+        <v>546</v>
+      </c>
+      <c r="E375" t="s">
+        <v>559</v>
+      </c>
+      <c r="F375">
+        <v>1</v>
+      </c>
+      <c r="G375">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="376" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A376" t="s">
+        <v>11</v>
+      </c>
+      <c r="B376" s="5">
+        <v>45189</v>
+      </c>
+      <c r="C376" t="s">
+        <v>610</v>
+      </c>
+      <c r="D376" s="4" t="s">
+        <v>546</v>
+      </c>
+      <c r="E376" t="s">
+        <v>559</v>
+      </c>
+      <c r="F376">
+        <v>1</v>
+      </c>
+      <c r="G376">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="377" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A377" t="s">
+        <v>560</v>
+      </c>
+      <c r="B377" s="5">
+        <v>45194</v>
+      </c>
+      <c r="C377" t="s">
+        <v>431</v>
+      </c>
+      <c r="D377" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="E377" t="s">
+        <v>561</v>
+      </c>
+      <c r="F377">
+        <v>1</v>
+      </c>
+      <c r="G377">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="378" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A378" t="s">
+        <v>560</v>
+      </c>
+      <c r="B378" s="5">
+        <v>45195</v>
+      </c>
+      <c r="C378" t="s">
+        <v>431</v>
+      </c>
+      <c r="D378" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="E378" t="s">
+        <v>561</v>
+      </c>
+      <c r="F378">
+        <v>1</v>
+      </c>
+      <c r="G378">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="379" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A379" t="s">
+        <v>560</v>
+      </c>
+      <c r="B379" s="5">
+        <v>45196</v>
+      </c>
+      <c r="C379" t="s">
+        <v>431</v>
+      </c>
+      <c r="D379" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="E379" t="s">
+        <v>561</v>
+      </c>
+      <c r="F379">
+        <v>1</v>
+      </c>
+      <c r="G379">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="380" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A380" t="s">
+        <v>560</v>
+      </c>
+      <c r="B380" s="5">
+        <v>45197</v>
+      </c>
+      <c r="C380" t="s">
+        <v>431</v>
+      </c>
+      <c r="D380" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="E380" t="s">
+        <v>561</v>
+      </c>
+      <c r="F380">
+        <v>1</v>
+      </c>
+      <c r="G380">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="381" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A381" t="s">
+        <v>560</v>
+      </c>
+      <c r="B381" s="5">
+        <v>45198</v>
+      </c>
+      <c r="C381" t="s">
+        <v>431</v>
+      </c>
+      <c r="D381" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="E381" t="s">
+        <v>561</v>
+      </c>
+      <c r="F381">
+        <v>1</v>
+      </c>
+      <c r="G381">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="382" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A382" t="s">
+        <v>560</v>
+      </c>
+      <c r="B382" s="5">
+        <v>45199</v>
+      </c>
+      <c r="C382" t="s">
+        <v>431</v>
+      </c>
+      <c r="D382" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="E382" t="s">
+        <v>561</v>
+      </c>
+      <c r="F382">
+        <v>1</v>
+      </c>
+      <c r="G382">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="383" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A383" t="s">
+        <v>560</v>
+      </c>
+      <c r="B383" s="5">
+        <v>45200</v>
+      </c>
+      <c r="C383" t="s">
+        <v>431</v>
+      </c>
+      <c r="D383" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="E383" t="s">
+        <v>561</v>
+      </c>
+      <c r="F383">
+        <v>1</v>
+      </c>
+      <c r="G383">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="384" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A384" t="s">
+        <v>560</v>
+      </c>
+      <c r="B384" s="5">
+        <v>45201</v>
+      </c>
+      <c r="C384" t="s">
+        <v>431</v>
+      </c>
+      <c r="D384" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="E384" t="s">
+        <v>561</v>
+      </c>
+      <c r="F384">
+        <v>1</v>
+      </c>
+      <c r="G384">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="385" spans="1:7" ht="15" customHeight="1">
+      <c r="A385" t="s">
+        <v>560</v>
+      </c>
+      <c r="B385" s="5">
+        <v>45202</v>
+      </c>
+      <c r="C385" t="s">
+        <v>431</v>
+      </c>
+      <c r="D385" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="E385" t="s">
+        <v>561</v>
+      </c>
+      <c r="F385">
+        <v>1</v>
+      </c>
+      <c r="G385">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="386" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A386" t="s">
+        <v>560</v>
+      </c>
+      <c r="B386" s="5">
+        <v>45203</v>
+      </c>
+      <c r="C386" t="s">
+        <v>431</v>
+      </c>
+      <c r="D386" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="E386" t="s">
+        <v>561</v>
+      </c>
+      <c r="F386">
+        <v>1</v>
+      </c>
+      <c r="G386">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="387" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A387" t="s">
+        <v>560</v>
+      </c>
+      <c r="B387" s="5">
+        <v>45204</v>
+      </c>
+      <c r="C387" t="s">
+        <v>431</v>
+      </c>
+      <c r="D387" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="E387" t="s">
+        <v>561</v>
+      </c>
+      <c r="F387">
+        <v>1</v>
+      </c>
+      <c r="G387">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="388" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A388" t="s">
+        <v>560</v>
+      </c>
+      <c r="B388" s="5">
+        <v>45205</v>
+      </c>
+      <c r="C388" t="s">
+        <v>431</v>
+      </c>
+      <c r="D388" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="E388" t="s">
+        <v>561</v>
+      </c>
+      <c r="F388">
+        <v>1</v>
+      </c>
+      <c r="G388">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="389" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A389" t="s">
+        <v>562</v>
+      </c>
+      <c r="B389" s="5">
+        <v>45195</v>
+      </c>
+      <c r="C389" t="s">
+        <v>613</v>
+      </c>
+      <c r="D389" s="4" t="s">
+        <v>546</v>
+      </c>
+      <c r="E389" t="s">
+        <v>563</v>
+      </c>
+      <c r="F389">
+        <v>1</v>
+      </c>
+      <c r="G389">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="390" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A390" t="s">
+        <v>564</v>
+      </c>
+      <c r="B390" s="5">
+        <v>45203</v>
+      </c>
+      <c r="C390" t="s">
+        <v>613</v>
+      </c>
+      <c r="D390" s="4" t="s">
+        <v>546</v>
+      </c>
+      <c r="E390" t="s">
+        <v>565</v>
+      </c>
+      <c r="F390">
+        <v>2</v>
+      </c>
+      <c r="G390">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="391" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A391" t="s">
+        <v>566</v>
+      </c>
+      <c r="B391" s="5">
+        <v>45227</v>
+      </c>
+      <c r="C391" t="s">
+        <v>533</v>
+      </c>
+      <c r="D391" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="E391" t="s">
+        <v>567</v>
+      </c>
+      <c r="F391">
+        <v>15</v>
+      </c>
+      <c r="G391">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="392" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A392" t="s">
+        <v>568</v>
+      </c>
+      <c r="B392" s="5">
+        <v>45238</v>
+      </c>
+      <c r="C392" t="s">
+        <v>96</v>
+      </c>
+      <c r="D392" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="E392" t="s">
+        <v>567</v>
+      </c>
+      <c r="F392">
+        <v>21</v>
+      </c>
+      <c r="G392">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="393" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A393" t="s">
+        <v>580</v>
+      </c>
+      <c r="B393" s="5">
+        <v>45239</v>
+      </c>
+      <c r="C393" s="17" t="s">
+        <v>581</v>
+      </c>
+      <c r="D393" s="16" t="s">
+        <v>547</v>
+      </c>
+      <c r="E393" t="s">
+        <v>567</v>
+      </c>
+      <c r="F393">
+        <v>14</v>
+      </c>
+      <c r="G393">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="394" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A394" t="s">
+        <v>569</v>
+      </c>
+      <c r="B394" s="5">
+        <v>45261</v>
+      </c>
+      <c r="C394" t="s">
+        <v>570</v>
+      </c>
+      <c r="D394" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="E394" t="s">
+        <v>567</v>
+      </c>
+      <c r="F394">
+        <v>20</v>
+      </c>
+      <c r="G394">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="395" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A395" t="s">
+        <v>582</v>
+      </c>
+      <c r="B395" s="5">
+        <v>45267</v>
+      </c>
+      <c r="C395" t="s">
+        <v>610</v>
+      </c>
+      <c r="D395" s="16" t="s">
+        <v>546</v>
+      </c>
+      <c r="E395" t="s">
+        <v>585</v>
+      </c>
+      <c r="F395">
+        <v>1</v>
+      </c>
+      <c r="G395">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="396" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A396" t="s">
+        <v>584</v>
+      </c>
+      <c r="B396" s="5">
+        <v>45267</v>
+      </c>
+      <c r="C396" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="D396" s="16" t="s">
+        <v>547</v>
+      </c>
+      <c r="E396" t="s">
+        <v>567</v>
+      </c>
+      <c r="F396">
+        <v>14</v>
+      </c>
+      <c r="G396">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="397" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A397" t="s">
+        <v>361</v>
+      </c>
+      <c r="B397" s="5">
+        <v>45268</v>
+      </c>
+      <c r="C397" s="17" t="s">
+        <v>586</v>
+      </c>
+      <c r="D397" s="16" t="s">
+        <v>545</v>
+      </c>
+      <c r="E397" t="s">
+        <v>587</v>
+      </c>
+      <c r="F397">
+        <v>1</v>
+      </c>
+      <c r="G397">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="398" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A398" t="s">
+        <v>353</v>
+      </c>
+      <c r="B398" s="5">
+        <v>45272</v>
+      </c>
+      <c r="C398" s="17" t="s">
+        <v>588</v>
+      </c>
+      <c r="D398" s="16" t="s">
+        <v>545</v>
+      </c>
+      <c r="E398" t="s">
+        <v>589</v>
+      </c>
+      <c r="F398">
+        <v>1</v>
+      </c>
+      <c r="G398">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="399" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A399" t="s">
+        <v>583</v>
+      </c>
+      <c r="B399" s="5">
+        <v>45278</v>
+      </c>
+      <c r="C399" s="18" t="s">
+        <v>614</v>
+      </c>
+      <c r="D399" s="16" t="s">
+        <v>545</v>
+      </c>
+      <c r="F399">
+        <v>1</v>
+      </c>
+      <c r="G399">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="400" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A400" t="s">
+        <v>583</v>
+      </c>
+      <c r="B400" s="5">
+        <v>45279</v>
+      </c>
+      <c r="C400" s="18" t="s">
+        <v>614</v>
+      </c>
+      <c r="D400" s="16" t="s">
+        <v>545</v>
+      </c>
+      <c r="F400">
+        <v>1</v>
+      </c>
+      <c r="G400">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="401" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A401" t="s">
+        <v>583</v>
+      </c>
+      <c r="B401" s="5">
+        <v>45280</v>
+      </c>
+      <c r="C401" s="18" t="s">
+        <v>614</v>
+      </c>
+      <c r="D401" s="16" t="s">
+        <v>545</v>
+      </c>
+      <c r="F401">
+        <v>1</v>
+      </c>
+      <c r="G401">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="402" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A402" t="s">
+        <v>590</v>
+      </c>
+      <c r="B402" s="5">
+        <v>45303</v>
+      </c>
+      <c r="C402" t="s">
+        <v>592</v>
+      </c>
+      <c r="D402" s="16" t="s">
+        <v>545</v>
+      </c>
+      <c r="E402" s="17" t="s">
+        <v>593</v>
+      </c>
+      <c r="F402">
+        <v>1</v>
+      </c>
+      <c r="G402">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="403" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A403" t="s">
+        <v>591</v>
+      </c>
+      <c r="B403" s="5">
+        <v>45303</v>
+      </c>
+      <c r="C403" t="s">
+        <v>609</v>
+      </c>
+      <c r="D403" s="16" t="s">
+        <v>547</v>
+      </c>
+      <c r="E403" s="17" t="s">
+        <v>567</v>
+      </c>
+      <c r="F403">
+        <v>4</v>
+      </c>
+      <c r="G403">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="404" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A404" t="s">
+        <v>594</v>
+      </c>
+      <c r="B404" s="5">
+        <v>45311</v>
+      </c>
+      <c r="C404" s="17" t="s">
+        <v>595</v>
+      </c>
+      <c r="D404" s="16" t="s">
+        <v>547</v>
+      </c>
+      <c r="E404" s="17" t="s">
+        <v>567</v>
+      </c>
+      <c r="F404">
+        <v>20</v>
+      </c>
+      <c r="G404">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="405" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A405" t="s">
+        <v>596</v>
+      </c>
+      <c r="B405" s="5">
+        <v>45321</v>
+      </c>
+      <c r="C405" s="17" t="s">
+        <v>597</v>
+      </c>
+      <c r="D405" s="16" t="s">
+        <v>545</v>
+      </c>
+      <c r="E405" s="17" t="s">
+        <v>598</v>
+      </c>
+      <c r="F405">
+        <v>1</v>
+      </c>
+      <c r="G405">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="406" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A406" t="s">
+        <v>599</v>
+      </c>
+      <c r="B406" s="5">
+        <v>45324</v>
+      </c>
+      <c r="C406" s="18" t="s">
+        <v>610</v>
+      </c>
+      <c r="D406" s="16" t="s">
+        <v>546</v>
+      </c>
+      <c r="E406" s="17" t="s">
+        <v>600</v>
+      </c>
+      <c r="F406">
+        <v>2</v>
+      </c>
+      <c r="G406">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="407" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A407" t="s">
+        <v>601</v>
+      </c>
+      <c r="B407" s="5">
+        <v>45331</v>
+      </c>
+      <c r="C407" s="18" t="s">
+        <v>610</v>
+      </c>
+      <c r="D407" s="16" t="s">
+        <v>546</v>
+      </c>
+      <c r="E407" s="17" t="s">
+        <v>602</v>
+      </c>
+      <c r="F407">
+        <v>1</v>
+      </c>
+      <c r="G407">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="408" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A408" t="s">
+        <v>482</v>
+      </c>
+      <c r="B408" s="5">
+        <v>45334</v>
+      </c>
+      <c r="C408" s="18" t="s">
+        <v>614</v>
+      </c>
+      <c r="D408" s="16" t="s">
+        <v>545</v>
+      </c>
+      <c r="E408" s="17" t="s">
+        <v>603</v>
+      </c>
+      <c r="F408">
+        <v>1</v>
+      </c>
+      <c r="G408">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="409" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A409" t="s">
+        <v>604</v>
+      </c>
+      <c r="B409" s="5">
+        <v>45355</v>
+      </c>
+      <c r="C409" s="18" t="s">
+        <v>615</v>
+      </c>
+      <c r="D409" s="16" t="s">
+        <v>547</v>
+      </c>
+      <c r="E409" s="17" t="s">
+        <v>567</v>
+      </c>
+      <c r="F409">
+        <v>15</v>
+      </c>
+      <c r="G409">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="410" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A410" t="s">
+        <v>605</v>
+      </c>
+      <c r="B410" s="5">
+        <v>45362</v>
+      </c>
+      <c r="C410" s="17" t="s">
+        <v>525</v>
+      </c>
+      <c r="D410" s="16" t="s">
+        <v>547</v>
+      </c>
+      <c r="E410" s="17" t="s">
+        <v>567</v>
+      </c>
+      <c r="F410">
+        <v>14</v>
+      </c>
+      <c r="G410">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="411" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A411" t="s">
+        <v>606</v>
+      </c>
+      <c r="B411" s="5">
+        <v>45342</v>
+      </c>
+      <c r="C411" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D411" s="16" t="s">
+        <v>547</v>
+      </c>
+      <c r="E411" s="17" t="s">
+        <v>567</v>
+      </c>
+      <c r="F411" s="13">
+        <v>10</v>
+      </c>
+      <c r="G411">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="412" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A412" t="s">
+        <v>607</v>
+      </c>
+      <c r="B412" s="5">
+        <v>45344</v>
+      </c>
+      <c r="C412" s="18" t="s">
+        <v>616</v>
+      </c>
+      <c r="D412" s="16" t="s">
+        <v>547</v>
+      </c>
+      <c r="E412" s="17" t="s">
+        <v>608</v>
+      </c>
+      <c r="F412" s="13">
+        <v>4</v>
+      </c>
+      <c r="G412">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="413" spans="1:7" ht="15.75" customHeight="1">
       <c r="B413" s="5"/>
     </row>
-    <row r="414" spans="2:2" ht="15.75" customHeight="1">
+    <row r="414" spans="1:7" ht="15.75" customHeight="1">
       <c r="B414" s="5"/>
     </row>
-    <row r="415" spans="2:2" ht="15.75" customHeight="1">
+    <row r="415" spans="1:7" ht="15.75" customHeight="1">
       <c r="B415" s="5"/>
     </row>
-    <row r="416" spans="2:2" ht="15.75" customHeight="1">
+    <row r="416" spans="1:7" ht="15.75" customHeight="1">
       <c r="B416" s="5"/>
     </row>
     <row r="417" spans="2:2" ht="15.75" customHeight="1">
@@ -12771,8 +13985,28 @@
     <row r="1011" spans="2:2" ht="15.75" customHeight="1">
       <c r="B1011" s="5"/>
     </row>
+    <row r="1012" spans="2:2" ht="15.75" customHeight="1">
+      <c r="B1012" s="5"/>
+    </row>
+    <row r="1013" spans="2:2" ht="15.75" customHeight="1">
+      <c r="B1013" s="5"/>
+    </row>
+    <row r="1014" spans="2:2" ht="15.75" customHeight="1">
+      <c r="B1014" s="5"/>
+    </row>
+    <row r="1015" spans="2:2" ht="15.75" customHeight="1">
+      <c r="B1015" s="5"/>
+    </row>
+    <row r="1016" spans="2:2" ht="15.75" customHeight="1">
+      <c r="B1016" s="5"/>
+    </row>
+    <row r="1017" spans="2:2" ht="15.75" customHeight="1">
+      <c r="B1017" s="5"/>
+    </row>
+    <row r="1018" spans="2:2" ht="15.75" customHeight="1">
+      <c r="B1018" s="5"/>
+    </row>
   </sheetData>
-  <autoFilter ref="F1:F1011" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>